<commit_message>
Updated README and data files
</commit_message>
<xml_diff>
--- a/Data/study_participant_list_anonymous.xlsx
+++ b/Data/study_participant_list_anonymous.xlsx
@@ -94,9 +94,6 @@
     <t>Unique IP Addresses Mobile Apps &amp; Web</t>
   </si>
   <si>
-    <t>Anonymous ID</t>
-  </si>
-  <si>
     <t>Shared Desktop Device</t>
   </si>
   <si>
@@ -116,6 +113,9 @@
   </si>
   <si>
     <t>3rd Quartile</t>
+  </si>
+  <si>
+    <t>User ID (Primary Key)</t>
   </si>
 </sst>
 </file>
@@ -970,7 +970,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E7" sqref="E7"/>
+      <selection pane="topRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -984,7 +984,7 @@
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="B1" t="s">
         <v>4</v>
@@ -1059,10 +1059,10 @@
         <v>3</v>
       </c>
       <c r="Z1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" t="s">
         <v>26</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.35">
@@ -11992,7 +11992,7 @@
     </row>
     <row r="129" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B129">
         <f>SUM(B2:B127)/Q129</f>
@@ -12101,7 +12101,7 @@
     </row>
     <row r="130" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B130">
         <f>_xlfn.STDEV.P(B2:B126)</f>
@@ -12166,7 +12166,7 @@
     </row>
     <row r="131" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B131">
         <f>MEDIAN(B2:B126)</f>
@@ -12231,7 +12231,7 @@
     </row>
     <row r="132" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B132">
         <f>QUARTILE(B2:B126,1)</f>
@@ -12296,7 +12296,7 @@
     </row>
     <row r="133" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B133">
         <f>QUARTILE(B2:B126,3)</f>

</xml_diff>